<commit_message>
Atualização de bug na data
A última data do agregado é o dia de hoje (que foi feita a requisição), com referência no dia útil imediatamente anterior
</commit_message>
<xml_diff>
--- a/Percentual - Títulos Públicos em Poder do Público(fonte).xlsx
+++ b/Percentual - Títulos Públicos em Poder do Público(fonte).xlsx
@@ -16,7 +16,7 @@
     <sheet name="Ref_31_08_2020" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Ref_30_09_2020" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Ref_30_10_2020" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Ref_13_11_2020" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Ref_23_11_2020" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Acum_6_meses" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Acum_12_meses" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
@@ -6533,10 +6533,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44150</v>
+        <v>44180</v>
       </c>
       <c r="B2" t="n">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -6544,32 +6544,32 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44180</v>
+        <v>44197</v>
       </c>
       <c r="B3" t="n">
-        <v>58</v>
+        <v>104419</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44197</v>
+        <v>44211</v>
       </c>
       <c r="B4" t="n">
-        <v>104129</v>
+        <v>68</v>
       </c>
       <c r="C4" t="n">
-        <v>2.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44211</v>
+        <v>44242</v>
       </c>
       <c r="B5" t="n">
-        <v>69</v>
+        <v>187</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -6577,98 +6577,98 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44242</v>
+        <v>44256</v>
       </c>
       <c r="B6" t="n">
-        <v>187</v>
+        <v>184000</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44256</v>
+        <v>44270</v>
       </c>
       <c r="B7" t="n">
-        <v>183929</v>
+        <v>56</v>
       </c>
       <c r="C7" t="n">
-        <v>4.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44270</v>
+        <v>44287</v>
       </c>
       <c r="B8" t="n">
-        <v>57</v>
+        <v>335016</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44287</v>
+        <v>44301</v>
       </c>
       <c r="B9" t="n">
-        <v>334961</v>
+        <v>64</v>
       </c>
       <c r="C9" t="n">
-        <v>7.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>44301</v>
+        <v>44331</v>
       </c>
       <c r="B10" t="n">
-        <v>65</v>
+        <v>74499</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>44331</v>
+        <v>44362</v>
       </c>
       <c r="B11" t="n">
-        <v>76108</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>1.73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>44362</v>
+        <v>44378</v>
       </c>
       <c r="B12" t="n">
-        <v>50</v>
+        <v>83102</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>44378</v>
+        <v>44392</v>
       </c>
       <c r="B13" t="n">
-        <v>82923</v>
+        <v>56</v>
       </c>
       <c r="C13" t="n">
-        <v>1.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>44392</v>
+        <v>44423</v>
       </c>
       <c r="B14" t="n">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -6676,54 +6676,54 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>44423</v>
+        <v>44440</v>
       </c>
       <c r="B15" t="n">
-        <v>176</v>
+        <v>228828</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>44440</v>
+        <v>44454</v>
       </c>
       <c r="B16" t="n">
-        <v>228726</v>
+        <v>47</v>
       </c>
       <c r="C16" t="n">
-        <v>5.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>44454</v>
+        <v>44470</v>
       </c>
       <c r="B17" t="n">
-        <v>48</v>
+        <v>162862</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>44470</v>
+        <v>44484</v>
       </c>
       <c r="B18" t="n">
-        <v>139622</v>
+        <v>55</v>
       </c>
       <c r="C18" t="n">
-        <v>3.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>44484</v>
+        <v>44515</v>
       </c>
       <c r="B19" t="n">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -6731,10 +6731,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>44515</v>
+        <v>44545</v>
       </c>
       <c r="B20" t="n">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -6742,32 +6742,32 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>44545</v>
+        <v>44562</v>
       </c>
       <c r="B21" t="n">
-        <v>40</v>
+        <v>74740</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>44562</v>
+        <v>44576</v>
       </c>
       <c r="B22" t="n">
-        <v>74594</v>
+        <v>49</v>
       </c>
       <c r="C22" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>44576</v>
+        <v>44607</v>
       </c>
       <c r="B23" t="n">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -6775,54 +6775,54 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>44607</v>
+        <v>44621</v>
       </c>
       <c r="B24" t="n">
-        <v>163</v>
+        <v>120945</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>44621</v>
+        <v>44635</v>
       </c>
       <c r="B25" t="n">
-        <v>117227</v>
+        <v>40</v>
       </c>
       <c r="C25" t="n">
-        <v>2.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>44635</v>
+        <v>44652</v>
       </c>
       <c r="B26" t="n">
-        <v>41</v>
+        <v>57466</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>44652</v>
+        <v>44666</v>
       </c>
       <c r="B27" t="n">
-        <v>57408</v>
+        <v>47</v>
       </c>
       <c r="C27" t="n">
-        <v>1.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>44666</v>
+        <v>44696</v>
       </c>
       <c r="B28" t="n">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -6830,10 +6830,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>44696</v>
+        <v>44727</v>
       </c>
       <c r="B29" t="n">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -6841,87 +6841,87 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>44727</v>
+        <v>44743</v>
       </c>
       <c r="B30" t="n">
-        <v>33</v>
+        <v>64515</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>44743</v>
+        <v>44757</v>
       </c>
       <c r="B31" t="n">
-        <v>64377</v>
+        <v>42</v>
       </c>
       <c r="C31" t="n">
-        <v>1.46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>44757</v>
+        <v>44788</v>
       </c>
       <c r="B32" t="n">
-        <v>42</v>
+        <v>147364</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>44788</v>
+        <v>44805</v>
       </c>
       <c r="B33" t="n">
-        <v>146113</v>
+        <v>129686</v>
       </c>
       <c r="C33" t="n">
-        <v>3.32</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>44805</v>
+        <v>44819</v>
       </c>
       <c r="B34" t="n">
-        <v>129626</v>
+        <v>35</v>
       </c>
       <c r="C34" t="n">
-        <v>2.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>44819</v>
+        <v>44835</v>
       </c>
       <c r="B35" t="n">
-        <v>36</v>
+        <v>46562</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>44835</v>
+        <v>44849</v>
       </c>
       <c r="B36" t="n">
-        <v>44676</v>
+        <v>40</v>
       </c>
       <c r="C36" t="n">
-        <v>1.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>44849</v>
+        <v>44880</v>
       </c>
       <c r="B37" t="n">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -6929,10 +6929,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>44880</v>
+        <v>44910</v>
       </c>
       <c r="B38" t="n">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -6940,32 +6940,32 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>44910</v>
+        <v>44927</v>
       </c>
       <c r="B39" t="n">
-        <v>29</v>
+        <v>128402</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>44927</v>
+        <v>44941</v>
       </c>
       <c r="B40" t="n">
-        <v>128061</v>
+        <v>36</v>
       </c>
       <c r="C40" t="n">
-        <v>2.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>44941</v>
+        <v>44972</v>
       </c>
       <c r="B41" t="n">
-        <v>36</v>
+        <v>144</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -6973,32 +6973,32 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>44972</v>
+        <v>44986</v>
       </c>
       <c r="B42" t="n">
-        <v>143</v>
+        <v>156652</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>3.53</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>44986</v>
+        <v>45000</v>
       </c>
       <c r="B43" t="n">
-        <v>156626</v>
+        <v>46</v>
       </c>
       <c r="C43" t="n">
-        <v>3.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>45000</v>
+        <v>45031</v>
       </c>
       <c r="B44" t="n">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -7006,54 +7006,54 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>45031</v>
+        <v>45061</v>
       </c>
       <c r="B45" t="n">
-        <v>33</v>
+        <v>119961</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>45061</v>
+        <v>45092</v>
       </c>
       <c r="B46" t="n">
-        <v>122933</v>
+        <v>24</v>
       </c>
       <c r="C46" t="n">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45092</v>
+        <v>45108</v>
       </c>
       <c r="B47" t="n">
-        <v>24</v>
+        <v>114759</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>45108</v>
+        <v>45122</v>
       </c>
       <c r="B48" t="n">
-        <v>114572</v>
+        <v>30</v>
       </c>
       <c r="C48" t="n">
-        <v>2.61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>45122</v>
+        <v>45153</v>
       </c>
       <c r="B49" t="n">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -7061,32 +7061,32 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>45153</v>
+        <v>45170</v>
       </c>
       <c r="B50" t="n">
-        <v>135</v>
+        <v>98971</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>45170</v>
+        <v>45184</v>
       </c>
       <c r="B51" t="n">
-        <v>98927</v>
+        <v>25</v>
       </c>
       <c r="C51" t="n">
-        <v>2.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>45184</v>
+        <v>45214</v>
       </c>
       <c r="B52" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -7094,10 +7094,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>45214</v>
+        <v>45245</v>
       </c>
       <c r="B53" t="n">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -7105,10 +7105,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>45245</v>
+        <v>45275</v>
       </c>
       <c r="B54" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -7116,32 +7116,32 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>45275</v>
+        <v>45292</v>
       </c>
       <c r="B55" t="n">
-        <v>20</v>
+        <v>183742</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>4.14</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>45292</v>
+        <v>45306</v>
       </c>
       <c r="B56" t="n">
-        <v>175948</v>
+        <v>25</v>
       </c>
       <c r="C56" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>45306</v>
+        <v>45337</v>
       </c>
       <c r="B57" t="n">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -7149,54 +7149,54 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>45337</v>
+        <v>45352</v>
       </c>
       <c r="B58" t="n">
-        <v>128</v>
+        <v>125210</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>45352</v>
+        <v>45366</v>
       </c>
       <c r="B59" t="n">
-        <v>125153</v>
+        <v>21</v>
       </c>
       <c r="C59" t="n">
-        <v>2.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>45366</v>
+        <v>45397</v>
       </c>
       <c r="B60" t="n">
-        <v>22</v>
+        <v>19479</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="B61" t="n">
-        <v>19706</v>
+        <v>74</v>
       </c>
       <c r="C61" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45427</v>
+        <v>45458</v>
       </c>
       <c r="B62" t="n">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -7204,10 +7204,10 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45458</v>
+        <v>45474</v>
       </c>
       <c r="B63" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -7215,10 +7215,10 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45474</v>
+        <v>45488</v>
       </c>
       <c r="B64" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
@@ -7226,43 +7226,43 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45488</v>
+        <v>45519</v>
       </c>
       <c r="B65" t="n">
-        <v>21</v>
+        <v>107409</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45519</v>
+        <v>45536</v>
       </c>
       <c r="B66" t="n">
-        <v>106661</v>
+        <v>168649</v>
       </c>
       <c r="C66" t="n">
-        <v>2.43</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45536</v>
+        <v>45550</v>
       </c>
       <c r="B67" t="n">
-        <v>168572</v>
+        <v>17</v>
       </c>
       <c r="C67" t="n">
-        <v>3.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45550</v>
+        <v>45580</v>
       </c>
       <c r="B68" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -7270,10 +7270,10 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45580</v>
+        <v>45611</v>
       </c>
       <c r="B69" t="n">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -7281,10 +7281,10 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45611</v>
+        <v>45641</v>
       </c>
       <c r="B70" t="n">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
@@ -7292,32 +7292,32 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>45641</v>
+        <v>45658</v>
       </c>
       <c r="B71" t="n">
-        <v>14</v>
+        <v>102977</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>45658</v>
+        <v>45672</v>
       </c>
       <c r="B72" t="n">
-        <v>102729</v>
+        <v>17</v>
       </c>
       <c r="C72" t="n">
-        <v>2.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>45672</v>
+        <v>45703</v>
       </c>
       <c r="B73" t="n">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -7325,29 +7325,29 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>45703</v>
+        <v>45717</v>
       </c>
       <c r="B74" t="n">
-        <v>82</v>
+        <v>112227</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>2.53</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>45717</v>
+        <v>45731</v>
       </c>
       <c r="B75" t="n">
-        <v>112172</v>
+        <v>14</v>
       </c>
       <c r="C75" t="n">
-        <v>2.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>45731</v>
+        <v>45762</v>
       </c>
       <c r="B76" t="n">
         <v>15</v>
@@ -7358,32 +7358,32 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>45762</v>
+        <v>45792</v>
       </c>
       <c r="B77" t="n">
-        <v>15</v>
+        <v>74542</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>45792</v>
+        <v>45823</v>
       </c>
       <c r="B78" t="n">
-        <v>75315</v>
+        <v>11</v>
       </c>
       <c r="C78" t="n">
-        <v>1.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>45823</v>
+        <v>45839</v>
       </c>
       <c r="B79" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
@@ -7391,7 +7391,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>45839</v>
+        <v>45853</v>
       </c>
       <c r="B80" t="n">
         <v>14</v>
@@ -7402,10 +7402,10 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>45853</v>
+        <v>45884</v>
       </c>
       <c r="B81" t="n">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
@@ -7413,29 +7413,29 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>45884</v>
+        <v>45901</v>
       </c>
       <c r="B82" t="n">
-        <v>78</v>
+        <v>154944</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>45901</v>
+        <v>45915</v>
       </c>
       <c r="B83" t="n">
-        <v>154874</v>
+        <v>11</v>
       </c>
       <c r="C83" t="n">
-        <v>3.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>45915</v>
+        <v>45945</v>
       </c>
       <c r="B84" t="n">
         <v>12</v>
@@ -7446,10 +7446,10 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>45945</v>
+        <v>45976</v>
       </c>
       <c r="B85" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
@@ -7457,10 +7457,10 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>45976</v>
+        <v>46006</v>
       </c>
       <c r="B86" t="n">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
@@ -7468,32 +7468,32 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>46006</v>
+        <v>46023</v>
       </c>
       <c r="B87" t="n">
-        <v>8</v>
+        <v>2008</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>46023</v>
+        <v>46037</v>
       </c>
       <c r="B88" t="n">
-        <v>1965</v>
+        <v>11</v>
       </c>
       <c r="C88" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>46037</v>
+        <v>46068</v>
       </c>
       <c r="B89" t="n">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -7501,32 +7501,32 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>46068</v>
+        <v>46082</v>
       </c>
       <c r="B90" t="n">
-        <v>75</v>
+        <v>154437</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>46082</v>
+        <v>46096</v>
       </c>
       <c r="B91" t="n">
-        <v>154367</v>
+        <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>3.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>46096</v>
+        <v>46127</v>
       </c>
       <c r="B92" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C92" t="n">
         <v>0</v>
@@ -7534,10 +7534,10 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>46127</v>
+        <v>46157</v>
       </c>
       <c r="B93" t="n">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
@@ -7545,10 +7545,10 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>46157</v>
+        <v>46188</v>
       </c>
       <c r="B94" t="n">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
@@ -7556,10 +7556,10 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>46188</v>
+        <v>46204</v>
       </c>
       <c r="B95" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -7567,10 +7567,10 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>46204</v>
+        <v>46218</v>
       </c>
       <c r="B96" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
@@ -7578,43 +7578,43 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>46218</v>
+        <v>46249</v>
       </c>
       <c r="B97" t="n">
-        <v>9</v>
+        <v>45568</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>46249</v>
+        <v>46266</v>
       </c>
       <c r="B98" t="n">
-        <v>45084</v>
+        <v>42586</v>
       </c>
       <c r="C98" t="n">
-        <v>1.03</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>46266</v>
+        <v>46280</v>
       </c>
       <c r="B99" t="n">
-        <v>42567</v>
+        <v>8</v>
       </c>
       <c r="C99" t="n">
-        <v>0.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>46280</v>
+        <v>46310</v>
       </c>
       <c r="B100" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" t="n">
         <v>0</v>
@@ -7622,10 +7622,10 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>46310</v>
+        <v>46341</v>
       </c>
       <c r="B101" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
@@ -7633,10 +7633,10 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>46341</v>
+        <v>46371</v>
       </c>
       <c r="B102" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C102" t="n">
         <v>0</v>
@@ -7644,32 +7644,32 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>46371</v>
+        <v>46388</v>
       </c>
       <c r="B103" t="n">
-        <v>5</v>
+        <v>82414</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>46388</v>
+        <v>46402</v>
       </c>
       <c r="B104" t="n">
-        <v>80430</v>
+        <v>7</v>
       </c>
       <c r="C104" t="n">
-        <v>1.83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>46402</v>
+        <v>46433</v>
       </c>
       <c r="B105" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
@@ -7677,32 +7677,32 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>46433</v>
+        <v>46447</v>
       </c>
       <c r="B106" t="n">
-        <v>33</v>
+        <v>11209</v>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>46447</v>
+        <v>46461</v>
       </c>
       <c r="B107" t="n">
-        <v>10865</v>
+        <v>6</v>
       </c>
       <c r="C107" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>46461</v>
+        <v>46492</v>
       </c>
       <c r="B108" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108" t="n">
         <v>0</v>
@@ -7710,10 +7710,10 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>46492</v>
+        <v>46522</v>
       </c>
       <c r="B109" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C109" t="n">
         <v>0</v>
@@ -7721,10 +7721,10 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>46522</v>
+        <v>46553</v>
       </c>
       <c r="B110" t="n">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
@@ -7732,10 +7732,10 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>46553</v>
+        <v>46569</v>
       </c>
       <c r="B111" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C111" t="n">
         <v>0</v>
@@ -7743,10 +7743,10 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>46569</v>
+        <v>46583</v>
       </c>
       <c r="B112" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C112" t="n">
         <v>0</v>
@@ -7754,10 +7754,10 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>46583</v>
+        <v>46614</v>
       </c>
       <c r="B113" t="n">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C113" t="n">
         <v>0</v>
@@ -7765,10 +7765,10 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>46614</v>
+        <v>46645</v>
       </c>
       <c r="B114" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
@@ -7776,10 +7776,10 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>46645</v>
+        <v>46675</v>
       </c>
       <c r="B115" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
@@ -7787,10 +7787,10 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>46675</v>
+        <v>46706</v>
       </c>
       <c r="B116" t="n">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C116" t="n">
         <v>0</v>
@@ -7798,10 +7798,10 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>46706</v>
+        <v>46736</v>
       </c>
       <c r="B117" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
@@ -7809,10 +7809,10 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>46736</v>
+        <v>46753</v>
       </c>
       <c r="B118" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
@@ -7820,10 +7820,10 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>46753</v>
+        <v>46767</v>
       </c>
       <c r="B119" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C119" t="n">
         <v>0</v>
@@ -7831,10 +7831,10 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>46767</v>
+        <v>46798</v>
       </c>
       <c r="B120" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C120" t="n">
         <v>0</v>
@@ -7842,10 +7842,10 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>46798</v>
+        <v>46827</v>
       </c>
       <c r="B121" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C121" t="n">
         <v>0</v>
@@ -7853,10 +7853,10 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>46827</v>
+        <v>46858</v>
       </c>
       <c r="B122" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C122" t="n">
         <v>0</v>
@@ -7864,10 +7864,10 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>46858</v>
+        <v>46888</v>
       </c>
       <c r="B123" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
@@ -7875,10 +7875,10 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>46888</v>
+        <v>46919</v>
       </c>
       <c r="B124" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C124" t="n">
         <v>0</v>
@@ -7886,10 +7886,10 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>46919</v>
+        <v>46935</v>
       </c>
       <c r="B125" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
@@ -7897,10 +7897,10 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>46935</v>
+        <v>46949</v>
       </c>
       <c r="B126" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -7908,32 +7908,32 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>46949</v>
+        <v>46980</v>
       </c>
       <c r="B127" t="n">
-        <v>4</v>
+        <v>26959</v>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>46980</v>
+        <v>47011</v>
       </c>
       <c r="B128" t="n">
-        <v>26702</v>
+        <v>3</v>
       </c>
       <c r="C128" t="n">
-        <v>0.61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>47011</v>
+        <v>47041</v>
       </c>
       <c r="B129" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -7941,10 +7941,10 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>47041</v>
+        <v>47072</v>
       </c>
       <c r="B130" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -7952,10 +7952,10 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>47072</v>
+        <v>47102</v>
       </c>
       <c r="B131" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -7963,32 +7963,32 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>47102</v>
+        <v>47119</v>
       </c>
       <c r="B132" t="n">
+        <v>44190</v>
+      </c>
+      <c r="C132" t="n">
         <v>1</v>
-      </c>
-      <c r="C132" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>47119</v>
+        <v>47133</v>
       </c>
       <c r="B133" t="n">
-        <v>44103</v>
+        <v>3</v>
       </c>
       <c r="C133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>47133</v>
+        <v>47164</v>
       </c>
       <c r="B134" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C134" t="n">
         <v>0</v>
@@ -7996,10 +7996,10 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>47164</v>
+        <v>47192</v>
       </c>
       <c r="B135" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C135" t="n">
         <v>0</v>
@@ -8007,10 +8007,10 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>47192</v>
+        <v>47223</v>
       </c>
       <c r="B136" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C136" t="n">
         <v>0</v>
@@ -8018,10 +8018,10 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>47223</v>
+        <v>47253</v>
       </c>
       <c r="B137" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C137" t="n">
         <v>0</v>
@@ -8029,10 +8029,10 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>47253</v>
+        <v>47284</v>
       </c>
       <c r="B138" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C138" t="n">
         <v>0</v>
@@ -8040,10 +8040,10 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>47284</v>
+        <v>47314</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
@@ -8051,10 +8051,10 @@
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>47314</v>
+        <v>47345</v>
       </c>
       <c r="B140" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C140" t="n">
         <v>0</v>
@@ -8062,10 +8062,10 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>47345</v>
+        <v>47376</v>
       </c>
       <c r="B141" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C141" t="n">
         <v>0</v>
@@ -8073,10 +8073,10 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>47376</v>
+        <v>47406</v>
       </c>
       <c r="B142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142" t="n">
         <v>0</v>
@@ -8084,10 +8084,10 @@
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>47406</v>
+        <v>47437</v>
       </c>
       <c r="B143" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
@@ -8095,10 +8095,10 @@
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>47437</v>
+        <v>47467</v>
       </c>
       <c r="B144" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
@@ -8106,10 +8106,10 @@
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>47467</v>
+        <v>47484</v>
       </c>
       <c r="B145" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="C145" t="n">
         <v>0</v>
@@ -8117,10 +8117,10 @@
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>47484</v>
+        <v>47498</v>
       </c>
       <c r="B146" t="n">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="C146" t="n">
         <v>0</v>
@@ -8128,10 +8128,10 @@
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>47498</v>
+        <v>47529</v>
       </c>
       <c r="B147" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C147" t="n">
         <v>0</v>
@@ -8139,10 +8139,10 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>47529</v>
+        <v>47557</v>
       </c>
       <c r="B148" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C148" t="n">
         <v>0</v>
@@ -8150,10 +8150,10 @@
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>47557</v>
+        <v>47588</v>
       </c>
       <c r="B149" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C149" t="n">
         <v>0</v>
@@ -8161,10 +8161,10 @@
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>47588</v>
+        <v>47618</v>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C150" t="n">
         <v>0</v>
@@ -8172,10 +8172,10 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>47618</v>
+        <v>47649</v>
       </c>
       <c r="B151" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
@@ -8183,10 +8183,10 @@
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>47649</v>
+        <v>47679</v>
       </c>
       <c r="B152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C152" t="n">
         <v>0</v>
@@ -8194,32 +8194,32 @@
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>47679</v>
+        <v>47710</v>
       </c>
       <c r="B153" t="n">
-        <v>2</v>
+        <v>50417</v>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>47710</v>
+        <v>47741</v>
       </c>
       <c r="B154" t="n">
-        <v>49882</v>
+        <v>2</v>
       </c>
       <c r="C154" t="n">
-        <v>1.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>47741</v>
+        <v>47771</v>
       </c>
       <c r="B155" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C155" t="n">
         <v>0</v>
@@ -8227,10 +8227,10 @@
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>47771</v>
+        <v>47802</v>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C156" t="n">
         <v>0</v>
@@ -8238,10 +8238,10 @@
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>47802</v>
+        <v>47832</v>
       </c>
       <c r="B157" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C157" t="n">
         <v>0</v>
@@ -8249,32 +8249,32 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>47832</v>
+        <v>47849</v>
       </c>
       <c r="B158" t="n">
-        <v>0</v>
+        <v>78641</v>
       </c>
       <c r="C158" t="n">
-        <v>0</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>47849</v>
+        <v>47863</v>
       </c>
       <c r="B159" t="n">
-        <v>78056</v>
+        <v>2</v>
       </c>
       <c r="C159" t="n">
-        <v>1.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>47863</v>
+        <v>47894</v>
       </c>
       <c r="B160" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C160" t="n">
         <v>0</v>
@@ -8282,10 +8282,10 @@
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>47894</v>
+        <v>47922</v>
       </c>
       <c r="B161" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C161" t="n">
         <v>0</v>
@@ -8293,10 +8293,10 @@
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>47922</v>
+        <v>47953</v>
       </c>
       <c r="B162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162" t="n">
         <v>0</v>
@@ -8304,10 +8304,10 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>47953</v>
+        <v>47983</v>
       </c>
       <c r="B163" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C163" t="n">
         <v>0</v>
@@ -8315,10 +8315,10 @@
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>47983</v>
+        <v>48014</v>
       </c>
       <c r="B164" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C164" t="n">
         <v>0</v>
@@ -8326,10 +8326,10 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>48014</v>
+        <v>48044</v>
       </c>
       <c r="B165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C165" t="n">
         <v>0</v>
@@ -8337,10 +8337,10 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>48044</v>
+        <v>48075</v>
       </c>
       <c r="B166" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -8348,10 +8348,10 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>48075</v>
+        <v>48106</v>
       </c>
       <c r="B167" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C167" t="n">
         <v>0</v>
@@ -8359,10 +8359,10 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>48106</v>
+        <v>48136</v>
       </c>
       <c r="B168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C168" t="n">
         <v>0</v>
@@ -8370,10 +8370,10 @@
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>48136</v>
+        <v>48167</v>
       </c>
       <c r="B169" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C169" t="n">
         <v>0</v>
@@ -8381,10 +8381,10 @@
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>48167</v>
+        <v>48197</v>
       </c>
       <c r="B170" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="C170" t="n">
         <v>0</v>
@@ -8392,10 +8392,10 @@
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>48197</v>
+        <v>48228</v>
       </c>
       <c r="B171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C171" t="n">
         <v>0</v>
@@ -8403,10 +8403,10 @@
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>48228</v>
+        <v>48259</v>
       </c>
       <c r="B172" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C172" t="n">
         <v>0</v>
@@ -8414,10 +8414,10 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>48259</v>
+        <v>48288</v>
       </c>
       <c r="B173" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C173" t="n">
         <v>0</v>
@@ -8425,10 +8425,10 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>48288</v>
+        <v>48319</v>
       </c>
       <c r="B174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C174" t="n">
         <v>0</v>
@@ -8436,10 +8436,10 @@
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>48319</v>
+        <v>48349</v>
       </c>
       <c r="B175" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C175" t="n">
         <v>0</v>
@@ -8447,10 +8447,10 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>48349</v>
+        <v>48380</v>
       </c>
       <c r="B176" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C176" t="n">
         <v>0</v>
@@ -8458,10 +8458,10 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>48380</v>
+        <v>48410</v>
       </c>
       <c r="B177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C177" t="n">
         <v>0</v>
@@ -8469,10 +8469,10 @@
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>48410</v>
+        <v>48441</v>
       </c>
       <c r="B178" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C178" t="n">
         <v>0</v>
@@ -8480,10 +8480,10 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>48441</v>
+        <v>48472</v>
       </c>
       <c r="B179" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C179" t="n">
         <v>0</v>
@@ -8491,10 +8491,10 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>48472</v>
+        <v>48502</v>
       </c>
       <c r="B180" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C180" t="n">
         <v>0</v>
@@ -8502,10 +8502,10 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>48502</v>
+        <v>48533</v>
       </c>
       <c r="B181" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C181" t="n">
         <v>0</v>
@@ -8513,10 +8513,10 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>48533</v>
+        <v>48563</v>
       </c>
       <c r="B182" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C182" t="n">
         <v>0</v>
@@ -8524,10 +8524,10 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>48563</v>
+        <v>48594</v>
       </c>
       <c r="B183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" t="n">
         <v>0</v>
@@ -8535,10 +8535,10 @@
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>48594</v>
+        <v>48625</v>
       </c>
       <c r="B184" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C184" t="n">
         <v>0</v>
@@ -8546,10 +8546,10 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>48625</v>
+        <v>48653</v>
       </c>
       <c r="B185" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C185" t="n">
         <v>0</v>
@@ -8557,10 +8557,10 @@
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>48653</v>
+        <v>48684</v>
       </c>
       <c r="B186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" t="n">
         <v>0</v>
@@ -8568,10 +8568,10 @@
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>48684</v>
+        <v>48714</v>
       </c>
       <c r="B187" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C187" t="n">
         <v>0</v>
@@ -8579,10 +8579,10 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>48714</v>
+        <v>48745</v>
       </c>
       <c r="B188" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C188" t="n">
         <v>0</v>
@@ -8590,10 +8590,10 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>48745</v>
+        <v>48775</v>
       </c>
       <c r="B189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C189" t="n">
         <v>0</v>
@@ -8601,10 +8601,10 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>48775</v>
+        <v>48806</v>
       </c>
       <c r="B190" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C190" t="n">
         <v>0</v>
@@ -8612,10 +8612,10 @@
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>48806</v>
+        <v>48837</v>
       </c>
       <c r="B191" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C191" t="n">
         <v>0</v>
@@ -8623,10 +8623,10 @@
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>48837</v>
+        <v>48867</v>
       </c>
       <c r="B192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C192" t="n">
         <v>0</v>
@@ -8634,10 +8634,10 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>48867</v>
+        <v>48898</v>
       </c>
       <c r="B193" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C193" t="n">
         <v>0</v>
@@ -8645,10 +8645,10 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>48898</v>
+        <v>48928</v>
       </c>
       <c r="B194" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C194" t="n">
         <v>0</v>
@@ -8656,10 +8656,10 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>48928</v>
+        <v>48959</v>
       </c>
       <c r="B195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C195" t="n">
         <v>0</v>
@@ -8667,10 +8667,10 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>48959</v>
+        <v>48990</v>
       </c>
       <c r="B196" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C196" t="n">
         <v>0</v>
@@ -8678,10 +8678,10 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>48990</v>
+        <v>49018</v>
       </c>
       <c r="B197" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C197" t="n">
         <v>0</v>
@@ -8689,10 +8689,10 @@
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>49018</v>
+        <v>49049</v>
       </c>
       <c r="B198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C198" t="n">
         <v>0</v>
@@ -8700,10 +8700,10 @@
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>49049</v>
+        <v>49079</v>
       </c>
       <c r="B199" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C199" t="n">
         <v>0</v>
@@ -8711,10 +8711,10 @@
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>49079</v>
+        <v>49110</v>
       </c>
       <c r="B200" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C200" t="n">
         <v>0</v>
@@ -8722,10 +8722,10 @@
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>49110</v>
+        <v>49140</v>
       </c>
       <c r="B201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C201" t="n">
         <v>0</v>
@@ -8733,10 +8733,10 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>49140</v>
+        <v>49171</v>
       </c>
       <c r="B202" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C202" t="n">
         <v>0</v>
@@ -8744,10 +8744,10 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>49171</v>
+        <v>49202</v>
       </c>
       <c r="B203" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C203" t="n">
         <v>0</v>
@@ -8755,7 +8755,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>49202</v>
+        <v>49232</v>
       </c>
       <c r="B204" t="n">
         <v>0</v>
@@ -8766,10 +8766,10 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>49232</v>
+        <v>49263</v>
       </c>
       <c r="B205" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C205" t="n">
         <v>0</v>
@@ -8777,10 +8777,10 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>49263</v>
+        <v>49293</v>
       </c>
       <c r="B206" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C206" t="n">
         <v>0</v>
@@ -8788,7 +8788,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>49293</v>
+        <v>49324</v>
       </c>
       <c r="B207" t="n">
         <v>0</v>
@@ -8799,10 +8799,10 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>49324</v>
+        <v>49355</v>
       </c>
       <c r="B208" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C208" t="n">
         <v>0</v>
@@ -8810,10 +8810,10 @@
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>49355</v>
+        <v>49383</v>
       </c>
       <c r="B209" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C209" t="n">
         <v>0</v>
@@ -8821,7 +8821,7 @@
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>49383</v>
+        <v>49414</v>
       </c>
       <c r="B210" t="n">
         <v>0</v>
@@ -8832,32 +8832,32 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>49414</v>
+        <v>49444</v>
       </c>
       <c r="B211" t="n">
-        <v>0</v>
+        <v>79207</v>
       </c>
       <c r="C211" t="n">
-        <v>0</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>49444</v>
+        <v>49505</v>
       </c>
       <c r="B212" t="n">
-        <v>80589</v>
+        <v>0</v>
       </c>
       <c r="C212" t="n">
-        <v>1.83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>49505</v>
+        <v>49536</v>
       </c>
       <c r="B213" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C213" t="n">
         <v>0</v>
@@ -8865,10 +8865,10 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>49536</v>
+        <v>49567</v>
       </c>
       <c r="B214" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C214" t="n">
         <v>0</v>
@@ -8876,10 +8876,10 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>49567</v>
+        <v>49628</v>
       </c>
       <c r="B215" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C215" t="n">
         <v>0</v>
@@ -8887,10 +8887,10 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>49628</v>
+        <v>49689</v>
       </c>
       <c r="B216" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C216" t="n">
         <v>0</v>
@@ -8898,10 +8898,10 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>49689</v>
+        <v>49720</v>
       </c>
       <c r="B217" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C217" t="n">
         <v>0</v>
@@ -8909,10 +8909,10 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>49720</v>
+        <v>49749</v>
       </c>
       <c r="B218" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C218" t="n">
         <v>0</v>
@@ -8920,10 +8920,10 @@
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>49749</v>
+        <v>49810</v>
       </c>
       <c r="B219" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C219" t="n">
         <v>0</v>
@@ -8931,10 +8931,10 @@
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>49810</v>
+        <v>49871</v>
       </c>
       <c r="B220" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C220" t="n">
         <v>0</v>
@@ -8942,10 +8942,10 @@
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>49871</v>
+        <v>49902</v>
       </c>
       <c r="B221" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C221" t="n">
         <v>0</v>
@@ -8953,10 +8953,10 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>49902</v>
+        <v>49933</v>
       </c>
       <c r="B222" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C222" t="n">
         <v>0</v>
@@ -8964,10 +8964,10 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>49933</v>
+        <v>49994</v>
       </c>
       <c r="B223" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C223" t="n">
         <v>0</v>
@@ -8975,10 +8975,10 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>49994</v>
+        <v>50055</v>
       </c>
       <c r="B224" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C224" t="n">
         <v>0</v>
@@ -8986,10 +8986,10 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>50055</v>
+        <v>50086</v>
       </c>
       <c r="B225" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C225" t="n">
         <v>0</v>
@@ -8997,10 +8997,10 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>50086</v>
+        <v>50175</v>
       </c>
       <c r="B226" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C226" t="n">
         <v>0</v>
@@ -9008,10 +9008,10 @@
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>50175</v>
+        <v>50236</v>
       </c>
       <c r="B227" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C227" t="n">
         <v>0</v>
@@ -9019,10 +9019,10 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>50236</v>
+        <v>50267</v>
       </c>
       <c r="B228" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C228" t="n">
         <v>0</v>
@@ -9030,10 +9030,10 @@
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>50267</v>
+        <v>50359</v>
       </c>
       <c r="B229" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C229" t="n">
         <v>0</v>
@@ -9041,10 +9041,10 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>50359</v>
+        <v>50451</v>
       </c>
       <c r="B230" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C230" t="n">
         <v>0</v>
@@ -9052,10 +9052,10 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>50451</v>
+        <v>50540</v>
       </c>
       <c r="B231" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C231" t="n">
         <v>0</v>
@@ -9063,10 +9063,10 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>50540</v>
+        <v>50632</v>
       </c>
       <c r="B232" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C232" t="n">
         <v>0</v>
@@ -9074,10 +9074,10 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>50632</v>
+        <v>50724</v>
       </c>
       <c r="B233" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C233" t="n">
         <v>0</v>
@@ -9085,10 +9085,10 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>50724</v>
+        <v>50816</v>
       </c>
       <c r="B234" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C234" t="n">
         <v>0</v>
@@ -9096,10 +9096,10 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>50816</v>
+        <v>50905</v>
       </c>
       <c r="B235" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C235" t="n">
         <v>0</v>
@@ -9107,10 +9107,10 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>50905</v>
+        <v>50997</v>
       </c>
       <c r="B236" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C236" t="n">
         <v>0</v>
@@ -9118,10 +9118,10 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>50997</v>
+        <v>51089</v>
       </c>
       <c r="B237" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C237" t="n">
         <v>0</v>
@@ -9129,10 +9129,10 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>51089</v>
+        <v>51181</v>
       </c>
       <c r="B238" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C238" t="n">
         <v>0</v>
@@ -9140,10 +9140,10 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>51181</v>
+        <v>51271</v>
       </c>
       <c r="B239" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C239" t="n">
         <v>0</v>
@@ -9151,32 +9151,32 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>51271</v>
+        <v>51363</v>
       </c>
       <c r="B240" t="n">
-        <v>12</v>
+        <v>51757</v>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>51363</v>
+        <v>51455</v>
       </c>
       <c r="B241" t="n">
-        <v>51234</v>
+        <v>12</v>
       </c>
       <c r="C241" t="n">
-        <v>1.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>51455</v>
+        <v>51547</v>
       </c>
       <c r="B242" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C242" t="n">
         <v>0</v>
@@ -9184,10 +9184,10 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>51547</v>
+        <v>51636</v>
       </c>
       <c r="B243" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C243" t="n">
         <v>0</v>
@@ -9195,10 +9195,10 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>51636</v>
+        <v>51728</v>
       </c>
       <c r="B244" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C244" t="n">
         <v>0</v>
@@ -9206,10 +9206,10 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>51728</v>
+        <v>51820</v>
       </c>
       <c r="B245" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C245" t="n">
         <v>0</v>
@@ -9217,10 +9217,10 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>51820</v>
+        <v>51912</v>
       </c>
       <c r="B246" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C246" t="n">
         <v>0</v>
@@ -9228,10 +9228,10 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>51912</v>
+        <v>52001</v>
       </c>
       <c r="B247" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C247" t="n">
         <v>0</v>
@@ -9239,10 +9239,10 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>52001</v>
+        <v>52093</v>
       </c>
       <c r="B248" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C248" t="n">
         <v>0</v>
@@ -9250,10 +9250,10 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>52093</v>
+        <v>52185</v>
       </c>
       <c r="B249" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C249" t="n">
         <v>0</v>
@@ -9261,10 +9261,10 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>52185</v>
+        <v>52277</v>
       </c>
       <c r="B250" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C250" t="n">
         <v>0</v>
@@ -9272,10 +9272,10 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>52277</v>
+        <v>52366</v>
       </c>
       <c r="B251" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C251" t="n">
         <v>0</v>
@@ -9283,10 +9283,10 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>52366</v>
+        <v>52458</v>
       </c>
       <c r="B252" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C252" t="n">
         <v>0</v>
@@ -9294,10 +9294,10 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>52458</v>
+        <v>52550</v>
       </c>
       <c r="B253" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C253" t="n">
         <v>0</v>
@@ -9305,10 +9305,10 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>52550</v>
+        <v>52642</v>
       </c>
       <c r="B254" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C254" t="n">
         <v>0</v>
@@ -9316,10 +9316,10 @@
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>52642</v>
+        <v>52732</v>
       </c>
       <c r="B255" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C255" t="n">
         <v>0</v>
@@ -9327,10 +9327,10 @@
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>52732</v>
+        <v>52824</v>
       </c>
       <c r="B256" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C256" t="n">
         <v>0</v>
@@ -9338,10 +9338,10 @@
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>52824</v>
+        <v>52916</v>
       </c>
       <c r="B257" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C257" t="n">
         <v>0</v>
@@ -9349,10 +9349,10 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>52916</v>
+        <v>53008</v>
       </c>
       <c r="B258" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C258" t="n">
         <v>0</v>
@@ -9360,29 +9360,29 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>53008</v>
+        <v>53097</v>
       </c>
       <c r="B259" t="n">
-        <v>3</v>
+        <v>75766</v>
       </c>
       <c r="C259" t="n">
-        <v>0</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>53097</v>
+        <v>53189</v>
       </c>
       <c r="B260" t="n">
-        <v>77373</v>
+        <v>3</v>
       </c>
       <c r="C260" t="n">
-        <v>1.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>53189</v>
+        <v>53373</v>
       </c>
       <c r="B261" t="n">
         <v>3</v>
@@ -9393,7 +9393,7 @@
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>53373</v>
+        <v>53554</v>
       </c>
       <c r="B262" t="n">
         <v>3</v>
@@ -9404,7 +9404,7 @@
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>53554</v>
+        <v>53738</v>
       </c>
       <c r="B263" t="n">
         <v>3</v>
@@ -9415,7 +9415,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>53738</v>
+        <v>53919</v>
       </c>
       <c r="B264" t="n">
         <v>3</v>
@@ -9426,10 +9426,10 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>53919</v>
+        <v>54103</v>
       </c>
       <c r="B265" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C265" t="n">
         <v>0</v>
@@ -9437,7 +9437,7 @@
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>54103</v>
+        <v>54285</v>
       </c>
       <c r="B266" t="n">
         <v>2</v>
@@ -9448,7 +9448,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>54285</v>
+        <v>54469</v>
       </c>
       <c r="B267" t="n">
         <v>2</v>
@@ -9459,7 +9459,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>54469</v>
+        <v>54650</v>
       </c>
       <c r="B268" t="n">
         <v>2</v>
@@ -9470,7 +9470,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>54650</v>
+        <v>54834</v>
       </c>
       <c r="B269" t="n">
         <v>2</v>
@@ -9481,52 +9481,41 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>54834</v>
+        <v>55015</v>
       </c>
       <c r="B270" t="n">
-        <v>2</v>
+        <v>150931</v>
       </c>
       <c r="C270" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>55015</v>
+        <v>56749</v>
       </c>
       <c r="B271" t="n">
-        <v>149457</v>
+        <v>50973</v>
       </c>
       <c r="C271" t="n">
-        <v>3.4</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="1" t="n">
-        <v>56749</v>
-      </c>
+      <c r="A272" s="1"/>
       <c r="B272" t="n">
-        <v>50648</v>
+        <v>4433719</v>
       </c>
       <c r="C272" t="n">
-        <v>1.15</v>
+        <v>100</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1"/>
       <c r="B273" t="n">
-        <v>4394885</v>
+        <v>100</v>
       </c>
       <c r="C273" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" s="1"/>
-      <c r="B274" t="n">
-        <v>100</v>
-      </c>
-      <c r="C274" t="n">
         <v>100</v>
       </c>
     </row>
@@ -9634,10 +9623,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>44148</v>
+        <v>44158</v>
       </c>
       <c r="B12" t="n">
-        <v>14.18</v>
+        <v>15.75</v>
       </c>
     </row>
   </sheetData>
@@ -9744,10 +9733,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>44148</v>
+        <v>44158</v>
       </c>
       <c r="B12" t="n">
-        <v>26.18</v>
+        <v>26.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>